<commit_message>
Added Prediction model for subclasses
</commit_message>
<xml_diff>
--- a/HRAF_NLP/HRAF_MultiLabel_ThreeLargeClasses_kfoldsDemo/Model_Prediction_Performance.xlsx
+++ b/HRAF_NLP/HRAF_MultiLabel_ThreeLargeClasses_kfoldsDemo/Model_Prediction_Performance.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,72 +487,72 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>ChatGPT</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45386</v>
+        <v>45888</v>
       </c>
       <c r="C2" t="n">
-        <v>0.907</v>
+        <v>0.88</v>
       </c>
       <c r="D2" t="n">
-        <v>0.822</v>
+        <v>0.79</v>
       </c>
       <c r="E2" t="n">
-        <v>0.805</v>
+        <v>0.771</v>
       </c>
       <c r="F2" t="n">
-        <v>0.851</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>0.845</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>1820</v>
+        <v>1895</v>
       </c>
       <c r="I2" t="n">
-        <v>7277</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
+          <t>model: ChatGPT ThreeMainClassModel</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Lexical search</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45344</v>
+        <v>45510</v>
       </c>
       <c r="C3" t="n">
-        <v>0.871</v>
+        <v>0.8389999866485596</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.7300000190734863</v>
       </c>
       <c r="E3" t="n">
-        <v>0.793</v>
+        <v>0.7089999914169312</v>
       </c>
       <c r="F3" t="n">
-        <v>0.828</v>
+        <v>0.7699999809265137</v>
       </c>
       <c r="G3" t="n">
-        <v>0.824</v>
+        <v>0.5789999961853027</v>
       </c>
       <c r="H3" t="n">
-        <v>1085</v>
+        <v>1895</v>
       </c>
       <c r="I3" t="n">
-        <v>4340</v>
+        <v>7578</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>model: MultiLabel_ThreeLargeClasses, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
+          <t>Ngram 1</t>
         </is>
       </c>
     </row>
@@ -563,28 +563,28 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45344</v>
+        <v>45386</v>
       </c>
       <c r="C4" t="n">
-        <v>0.916</v>
+        <v>0.907</v>
       </c>
       <c r="D4" t="n">
-        <v>0.827</v>
+        <v>0.822</v>
       </c>
       <c r="E4" t="n">
-        <v>0.838</v>
+        <v>0.805</v>
       </c>
       <c r="F4" t="n">
-        <v>0.865</v>
+        <v>0.851</v>
       </c>
       <c r="G4" t="n">
-        <v>0.86</v>
+        <v>0.845</v>
       </c>
       <c r="H4" t="n">
-        <v>1085</v>
+        <v>1820</v>
       </c>
       <c r="I4" t="n">
-        <v>4340</v>
+        <v>7277</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -599,32 +599,32 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="C5" t="n">
-        <v>0.906</v>
+        <v>0.871</v>
       </c>
       <c r="D5" t="n">
-        <v>0.82</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8129999999999999</v>
+        <v>0.793</v>
       </c>
       <c r="F5" t="n">
-        <v>0.851</v>
+        <v>0.828</v>
       </c>
       <c r="G5" t="n">
-        <v>0.847</v>
+        <v>0.824</v>
       </c>
       <c r="H5" t="n">
-        <v>1123</v>
+        <v>1085</v>
       </c>
       <c r="I5" t="n">
-        <v>4491</v>
+        <v>4340</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
+          <t>model: MultiLabel_ThreeLargeClasses, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
         </is>
       </c>
     </row>
@@ -635,68 +635,68 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45337</v>
+        <v>45344</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9389999999999999</v>
+        <v>0.916</v>
       </c>
       <c r="D6" t="n">
-        <v>0.828</v>
+        <v>0.827</v>
       </c>
       <c r="E6" t="n">
-        <v>0.77</v>
+        <v>0.838</v>
       </c>
       <c r="F6" t="n">
-        <v>0.853</v>
+        <v>0.865</v>
       </c>
       <c r="G6" t="n">
-        <v>0.846</v>
+        <v>0.86</v>
       </c>
       <c r="H6" t="n">
-        <v>291</v>
+        <v>1085</v>
       </c>
       <c r="I6" t="n">
-        <v>1648</v>
+        <v>4340</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: ../HRAF_MultiLabel_ThreeLargeClasses/</t>
+          <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Lexical search</t>
+          <t>NLP</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45324</v>
+        <v>45338</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8199999928474426</v>
+        <v>0.906</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7379999756813049</v>
+        <v>0.82</v>
       </c>
       <c r="E7" t="n">
-        <v>0.656000018119812</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>0.75</v>
+        <v>0.851</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5529999732971191</v>
+        <v>0.847</v>
       </c>
       <c r="H7" t="n">
-        <v>728</v>
+        <v>1123</v>
       </c>
       <c r="I7" t="n">
-        <v>2910</v>
+        <v>4491</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Ngram 1</t>
+          <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
         </is>
       </c>
     </row>
@@ -707,30 +707,102 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
+        <v>45337</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.9389999999999999</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.828</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="H8" t="n">
+        <v>291</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1648</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: ../HRAF_MultiLabel_ThreeLargeClasses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Lexical search</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>45324</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C9" t="n">
+        <v>0.8199999928474426</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.7379999756813049</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.656000018119812</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.5529999732971191</v>
+      </c>
+      <c r="H9" t="n">
+        <v>728</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2910</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Ngram 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>NLP</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45324</v>
+      </c>
+      <c r="C10" t="n">
         <v>0.883</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D10" t="n">
         <v>0.8120000000000001</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E10" t="n">
         <v>0.733</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F10" t="n">
         <v>0.8159999999999999</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G10" t="n">
         <v>0.8090000000000001</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H10" t="n">
         <v>728</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I10" t="n">
         <v>2910</v>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>model: MultiLabel_ThreeLargeClasses_kfoldsDEMO, Dataset: MultiLabel_ThreeLargeClasses_kfoldsDEMO</t>
         </is>

</xml_diff>